<commit_message>
v2.03 & 25mm Trickler
</commit_message>
<xml_diff>
--- a/Hardware/RS232/Settings.xlsx
+++ b/Hardware/RS232/Settings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
   <si>
     <t xml:space="preserve">A&amp;D</t>
   </si>
@@ -31,7 +31,10 @@
     <t xml:space="preserve">KERN</t>
   </si>
   <si>
-    <t xml:space="preserve">Sartorius</t>
+    <t xml:space="preserve">Sartorius 9PIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sartorius 25PIN</t>
   </si>
   <si>
     <t xml:space="preserve">Steinberg</t>
@@ -46,6 +49,9 @@
     <t xml:space="preserve">RS_2</t>
   </si>
   <si>
+    <t xml:space="preserve">Bottom2&gt;Top4</t>
+  </si>
+  <si>
     <t xml:space="preserve">RS_3_R</t>
   </si>
   <si>
@@ -56,6 +62,27 @@
   </si>
   <si>
     <t xml:space="preserve">RS_5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Top4&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Bottom2</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">RXD</t>
@@ -86,7 +113,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -107,6 +134,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
       <family val="0"/>
     </font>
   </fonts>
@@ -152,8 +185,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -174,164 +215,193 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.43"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>6</v>
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>8</v>
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>6</v>
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>6</v>
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>6</v>
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>14</v>
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>13</v>
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>18</v>
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get Weight always from Scale
</commit_message>
<xml_diff>
--- a/Hardware/RS232/Settings.xlsx
+++ b/Hardware/RS232/Settings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="20">
   <si>
     <t xml:space="preserve">A&amp;D</t>
   </si>
@@ -49,9 +49,6 @@
     <t xml:space="preserve">RS_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Bottom2&gt;Top4</t>
-  </si>
-  <si>
     <t xml:space="preserve">RS_3_R</t>
   </si>
   <si>
@@ -62,27 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">RS_5</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Top4&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">Bottom2</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">RXD</t>
@@ -141,6 +117,7 @@
       <color rgb="FF000000"/>
       <name val="宋体"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -185,8 +162,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -218,190 +199,186 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>21</v>
+      <c r="D10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enclosure for Control Unit by marwaw-ops
https://github.com/ripper121/RoboTrickler/issues/3
https://github.com/marwaw-ops
</commit_message>
<xml_diff>
--- a/Hardware/RS232/Settings.xlsx
+++ b/Hardware/RS232/Settings.xlsx
@@ -31,16 +31,16 @@
     <t xml:space="preserve">KERN</t>
   </si>
   <si>
+    <t xml:space="preserve">Sartorius 9PIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sartorius 25PIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acculab 25PIN</t>
+  </si>
+  <si>
     <t xml:space="preserve">A&amp;D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sartorius 9PIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sartorius 25PIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acculab 25PIN</t>
   </si>
   <si>
     <t xml:space="preserve">RS_1</t>
@@ -307,14 +307,14 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="18.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="18.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -344,7 +344,7 @@
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -361,13 +361,13 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -375,7 +375,7 @@
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -392,13 +392,13 @@
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -406,7 +406,7 @@
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -423,13 +423,13 @@
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -450,13 +450,13 @@
         <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -476,13 +476,13 @@
         <v>16</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>